<commit_message>
Failing adjacency tests complete
</commit_message>
<xml_diff>
--- a/Assignments/C14A1_RunningRabbit_Ramirez/BoardTestLayout.xlsx
+++ b/Assignments/C14A1_RunningRabbit_Ramirez/BoardTestLayout.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shani\OneDrive - Colorado School of Mines\306CSCI\Clue-Game\Assignments\C14A1_RunningRabbit_Ramirez\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amiri\eclipse-workspace\CSCI306\Clue-Game\Assignments\C14A1_RunningRabbit_Ramirez\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{99E71423-8C67-45A6-AE24-F68AA2D13D6F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{1B5F2755-1BDC-4502-80AA-FFBEFF8D1D11}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEBC9986-F094-4295-B9EE-A3EBB663329E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13980" yWindow="600" windowWidth="21600" windowHeight="14415" xr2:uid="{92377532-FDB0-4122-9747-2A779DD21D57}"/>
+    <workbookView xWindow="18480" yWindow="2112" windowWidth="17280" windowHeight="8964" xr2:uid="{92377532-FDB0-4122-9747-2A779DD21D57}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="35">
   <si>
     <t>X</t>
   </si>
@@ -118,6 +118,24 @@
   </si>
   <si>
     <t>Test targets</t>
+  </si>
+  <si>
+    <t>W1</t>
+  </si>
+  <si>
+    <t>W6</t>
+  </si>
+  <si>
+    <t>W4</t>
+  </si>
+  <si>
+    <t>W2</t>
+  </si>
+  <si>
+    <t>WIR</t>
+  </si>
+  <si>
+    <t>Wir</t>
   </si>
 </sst>
 </file>
@@ -133,7 +151,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -194,6 +212,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -207,7 +231,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -221,6 +245,7 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -231,8 +256,8 @@
     <mruColors>
       <color rgb="FFFF5357"/>
       <color rgb="FF79DD79"/>
+      <color rgb="FFBD81FF"/>
       <color rgb="FF7EFAEE"/>
-      <color rgb="FFBD81FF"/>
       <color rgb="FFFF99FF"/>
       <color rgb="FFFFCCFF"/>
       <color rgb="FFFF8FA2"/>
@@ -550,15 +575,15 @@
   <dimension ref="A1:V31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="4.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="22" width="4.140625" customWidth="1"/>
+    <col min="1" max="22" width="4.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
         <v>6</v>
       </c>
@@ -580,7 +605,7 @@
       <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="8" t="s">
         <v>10</v>
       </c>
       <c r="I1" s="3" t="s">
@@ -589,8 +614,8 @@
       <c r="J1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="2" t="s">
-        <v>10</v>
+      <c r="K1" s="9" t="s">
+        <v>31</v>
       </c>
       <c r="L1" s="2" t="s">
         <v>10</v>
@@ -611,7 +636,7 @@
         <v>10</v>
       </c>
       <c r="R1" s="9" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="S1" s="3" t="s">
         <v>8</v>
@@ -626,7 +651,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
@@ -657,7 +682,7 @@
       <c r="J2" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="K2" s="8" t="s">
+      <c r="K2" s="2" t="s">
         <v>10</v>
       </c>
       <c r="L2" s="7" t="s">
@@ -694,7 +719,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
@@ -704,7 +729,7 @@
       <c r="C3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E3" s="3" t="s">
@@ -762,7 +787,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -830,7 +855,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
@@ -855,7 +880,7 @@
       <c r="H5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="I5" s="9" t="s">
+      <c r="I5" s="2" t="s">
         <v>10</v>
       </c>
       <c r="J5" s="2" t="s">
@@ -898,7 +923,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>6</v>
       </c>
@@ -966,7 +991,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
@@ -1034,7 +1059,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
@@ -1068,7 +1093,7 @@
       <c r="K8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L8" s="9" t="s">
+      <c r="L8" s="2" t="s">
         <v>10</v>
       </c>
       <c r="M8" s="2" t="s">
@@ -1096,13 +1121,13 @@
         <v>10</v>
       </c>
       <c r="U8" s="9" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="V8">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>10</v>
       </c>
@@ -1170,7 +1195,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>5</v>
       </c>
@@ -1184,7 +1209,7 @@
         <v>5</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>10</v>
@@ -1238,7 +1263,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>5</v>
       </c>
@@ -1276,15 +1301,15 @@
         <v>0</v>
       </c>
       <c r="M11" s="9" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="N11" s="2" t="s">
         <v>10</v>
       </c>
       <c r="O11" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="P11" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="P11" s="4" t="s">
         <v>15</v>
       </c>
       <c r="Q11" s="3" t="s">
@@ -1306,7 +1331,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>5</v>
       </c>
@@ -1322,7 +1347,7 @@
       <c r="E12" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="F12" s="9" t="s">
+      <c r="F12" s="2" t="s">
         <v>10</v>
       </c>
       <c r="G12" s="6" t="s">
@@ -1374,7 +1399,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>5</v>
       </c>
@@ -1426,7 +1451,7 @@
       <c r="Q13" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="R13" s="4" t="s">
+      <c r="R13" s="5" t="s">
         <v>14</v>
       </c>
       <c r="S13" s="3" t="s">
@@ -1442,7 +1467,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>5</v>
       </c>
@@ -1510,9 +1535,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>10</v>
@@ -1578,7 +1603,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>10</v>
       </c>
@@ -1646,7 +1671,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>10</v>
       </c>
@@ -1656,7 +1681,7 @@
       <c r="C17" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="D17" s="5" t="s">
         <v>11</v>
       </c>
       <c r="E17" s="7" t="s">
@@ -1714,7 +1739,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>4</v>
       </c>
@@ -1728,7 +1753,7 @@
         <v>4</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>10</v>
@@ -1782,7 +1807,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>4</v>
       </c>
@@ -1819,7 +1844,7 @@
       <c r="L19" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="M19" s="4" t="s">
+      <c r="M19" s="13" t="s">
         <v>12</v>
       </c>
       <c r="N19" s="5" t="s">
@@ -1850,7 +1875,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>4</v>
       </c>
@@ -1902,7 +1927,7 @@
       <c r="Q20" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="R20" s="9" t="s">
+      <c r="R20" s="4" t="s">
         <v>13</v>
       </c>
       <c r="S20" s="3" t="s">
@@ -1918,7 +1943,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>4</v>
       </c>
@@ -1986,7 +2011,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
         <v>4</v>
       </c>
@@ -2003,7 +2028,7 @@
         <v>10</v>
       </c>
       <c r="F22" s="9" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="G22" s="3" t="s">
         <v>3</v>
@@ -2054,7 +2079,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>0</v>
       </c>
@@ -2119,7 +2144,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A25" s="12" t="s">
         <v>22</v>
       </c>
@@ -2134,7 +2159,7 @@
       <c r="J25" s="12"/>
       <c r="K25" s="12"/>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.3">
       <c r="B26" s="11" t="s">
         <v>23</v>
       </c>
@@ -2150,7 +2175,7 @@
       <c r="L26" s="11"/>
       <c r="N26" s="6"/>
     </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A27" s="10"/>
       <c r="B27" s="11" t="s">
         <v>24</v>
@@ -2166,7 +2191,7 @@
       <c r="K27" s="11"/>
       <c r="L27" s="11"/>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A28" s="5"/>
       <c r="B28" s="11" t="s">
         <v>25</v>
@@ -2182,7 +2207,7 @@
       <c r="K28" s="11"/>
       <c r="L28" s="11"/>
     </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A29" s="7"/>
       <c r="B29" s="11" t="s">
         <v>26</v>
@@ -2198,7 +2223,7 @@
       <c r="K29" s="11"/>
       <c r="L29" s="11"/>
     </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A30" s="8"/>
       <c r="B30" s="11" t="s">
         <v>27</v>
@@ -2214,7 +2239,7 @@
       <c r="K30" s="11"/>
       <c r="L30" s="11"/>
     </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A31" s="9"/>
       <c r="B31" s="11" t="s">
         <v>28</v>
@@ -2246,21 +2271,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100ADA2F9109880964896E442C29DE38AC2" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="25242ce4e2c19792a6cc0dc442ea672f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="016359d3-cff7-42c2-aba4-99a986bb7b57" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="46a1a1061a183006076f95c247e0b4d4" ns3:_="">
     <xsd:import namespace="016359d3-cff7-42c2-aba4-99a986bb7b57"/>
@@ -2432,31 +2442,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8CAE1FB2-A462-49AE-934E-5B0D2C06BEEF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="016359d3-cff7-42c2-aba4-99a986bb7b57"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A64AB8DA-31AE-447A-9838-674F1CB263A9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{525F27A9-21A3-4685-9FFE-523C650D89BD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2472,4 +2473,28 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A64AB8DA-31AE-447A-9838-674F1CB263A9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8CAE1FB2-A462-49AE-934E-5B0D2C06BEEF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="016359d3-cff7-42c2-aba4-99a986bb7b57"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>